<commit_message>
auipc lui working, wip branch
</commit_message>
<xml_diff>
--- a/docs/Control path.xlsx
+++ b/docs/Control path.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{280BA75C-C463-4414-B0FF-94F49E4A72B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modulos_quartus\DM_Michel_Castillo_RISC_V\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C531E9-9D22-4185-8A7B-501BB9377C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="26">
   <si>
     <t>Instruction/Signals</t>
   </si>
@@ -54,9 +59,6 @@
     <t>ALUOp</t>
   </si>
   <si>
-    <t>ALUSrc</t>
-  </si>
-  <si>
     <t>RegWrite</t>
   </si>
   <si>
@@ -103,14 +105,28 @@
   </si>
   <si>
     <t>JAL</t>
+  </si>
+  <si>
+    <t>ALUSrcB</t>
+  </si>
+  <si>
+    <t>ALUSrcA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,8 +157,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,7 +177,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -457,27 +473,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K27"/>
+  <dimension ref="B2:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -503,333 +520,367 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:11">
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11">
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="J8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
+        <v>10</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
+        <v>11</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -839,8 +890,9 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="2:11">
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -850,8 +902,9 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="2:11">
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -861,8 +914,9 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="2:11">
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -872,8 +926,9 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="3:11">
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -883,8 +938,9 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="3:11">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -894,8 +950,9 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="3:11">
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -905,8 +962,9 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="3:11">
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -916,8 +974,9 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="3:11">
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -927,8 +986,9 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="3:11">
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -938,8 +998,9 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="3:11">
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -949,8 +1010,9 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="3:11">
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -960,8 +1022,9 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="3:11">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -971,8 +1034,9 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="3:11">
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -982,8 +1046,9 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="3:11">
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -993,8 +1058,10 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified control path excel
</commit_message>
<xml_diff>
--- a/docs/Control path.xlsx
+++ b/docs/Control path.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modulos_quartus\DM_Michel_Castillo_RISC_V\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C531E9-9D22-4185-8A7B-501BB9377C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90396BD-A732-4193-886F-21597BDBBBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="27">
   <si>
     <t>Instruction/Signals</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>ALUSrcA</t>
+  </si>
+  <si>
+    <t>JALR_o</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="B2:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,6 +531,9 @@
       <c r="L2" t="s">
         <v>8</v>
       </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -563,6 +569,9 @@
       <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -598,6 +607,9 @@
       <c r="L4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -633,6 +645,9 @@
       <c r="L5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -668,6 +683,9 @@
       <c r="L6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
@@ -704,6 +722,9 @@
       <c r="L7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M7" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -739,6 +760,9 @@
       <c r="L8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="M8" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -774,6 +798,9 @@
       <c r="L9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="M9" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -809,6 +836,9 @@
       <c r="L10" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M10" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -844,6 +874,9 @@
       <c r="L11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M11" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
@@ -878,6 +911,9 @@
       </c>
       <c r="L12" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">

</xml_diff>